<commit_message>
Commit: changed save ticket number
</commit_message>
<xml_diff>
--- a/BookingPortal/Files/export/AirBooking/du-lieu-xuat-ve.xlsx
+++ b/BookingPortal/Files/export/AirBooking/du-lieu-xuat-ve.xlsx
@@ -5,16 +5,16 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="T 2020-12" sheetId="1" r:id="rId1"/>
+    <sheet name="T 2021-01" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <si>
-    <t>DỮ LIỆU XUẤT VÉ 04/12/2020 - 04/12/2020</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+  <si>
+    <t>DỮ LIỆU XUẤT VÉ 11/01/2021 - 13/01/2021</t>
   </si>
   <si>
     <t>#</t>
@@ -83,25 +83,19 @@
     <t>Đơn vị</t>
   </si>
   <si>
-    <t>01-01-0001</t>
-  </si>
-  <si>
-    <t>00000000000001</t>
-  </si>
-  <si>
-    <t>NGUYEN HONG ANH</t>
-  </si>
-  <si>
-    <t>FOC</t>
-  </si>
-  <si>
-    <t>FL1</t>
+    <t>11-01-2021</t>
+  </si>
+  <si>
+    <t>PHUNG QUOC VIET</t>
+  </si>
+  <si>
+    <t>GIG</t>
   </si>
   <si>
     <t>Khách lẻ</t>
   </si>
   <si>
-    <t>dl01 tickting 01</t>
+    <t>Tô Đức Anh</t>
   </si>
   <si>
     <t>Nội địa</t>
@@ -113,22 +107,55 @@
     <t>1:SGN-HAN</t>
   </si>
   <si>
-    <t>24-12-2020</t>
+    <t>27-03-2021</t>
   </si>
   <si>
     <t>Khứ hồi</t>
   </si>
   <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>12-01-2021</t>
+  </si>
+  <si>
+    <t>1:HAN-SGN</t>
+  </si>
+  <si>
+    <t>25-03-2021</t>
+  </si>
+  <si>
+    <t>Một chiều</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>TO DUC ANH</t>
+  </si>
+  <si>
+    <t>BUI THI QUYEN</t>
+  </si>
+  <si>
     <t>P</t>
   </si>
   <si>
-    <t>VND</t>
-  </si>
-  <si>
-    <t>00000000000004</t>
-  </si>
-  <si>
-    <t>NGUYEN DUC ANH</t>
+    <t>7382405790441</t>
+  </si>
+  <si>
+    <t>7382405790442</t>
+  </si>
+  <si>
+    <t>13-01-2021</t>
+  </si>
+  <si>
+    <t>7382405816727</t>
+  </si>
+  <si>
+    <t>1:DLI-HAN</t>
+  </si>
+  <si>
+    <t>23-03-2021</t>
   </si>
 </sst>
 </file>
@@ -244,7 +271,7 @@
   <sheetPr>
     <tabColor rgb="FF000000"/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -252,17 +279,17 @@
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="12.6827850341797" customWidth="1"/>
-    <col min="3" max="3" width="16.7238941192627" customWidth="1"/>
-    <col min="4" max="4" width="19.5424385070801" customWidth="1"/>
+    <col min="3" max="3" width="15.6302366256714" customWidth="1"/>
+    <col min="4" max="4" width="18.2769069671631" customWidth="1"/>
     <col min="5" max="5" width="13.2239866256714" customWidth="1"/>
     <col min="6" max="6" width="9.4591064453125" customWidth="1"/>
     <col min="7" max="7" width="15.4726848602295" customWidth="1"/>
-    <col min="8" max="8" width="14.872145652771" customWidth="1"/>
+    <col min="8" max="8" width="13.4889612197876" customWidth="1"/>
     <col min="9" max="9" width="12.0249547958374" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="11.477614402771" customWidth="1"/>
     <col min="12" max="12" width="15.1002883911133" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.3563356399536" customWidth="1"/>
     <col min="14" max="14" width="9.140625" customWidth="1"/>
     <col min="15" max="15" width="9.24324035644531" customWidth="1"/>
     <col min="16" max="16" width="9.140625" customWidth="1"/>
@@ -417,134 +444,644 @@
       <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="N3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="O3" s="7">
-        <v>378000</v>
+        <v>718000</v>
       </c>
       <c r="P3" s="7">
-        <v>820000</v>
+        <v>940000</v>
       </c>
       <c r="Q3" s="7">
-        <v>38000</v>
+        <v>72000</v>
       </c>
       <c r="R3" s="7">
-        <v>120000</v>
+        <v>0</v>
       </c>
       <c r="S3" s="7">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="T3" s="7">
-        <v>150000</v>
+        <v>0</v>
       </c>
       <c r="U3" s="8">
-        <v>1606000</v>
-      </c>
-      <c r="V3" s="9" t="s">
-        <v>36</v>
-      </c>
+        <v>1730000</v>
+      </c>
+      <c r="V3" s="9"/>
     </row>
     <row r="4">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="N4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="O4" s="7">
+        <v>558000</v>
+      </c>
+      <c r="P4" s="7">
+        <v>820000</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>56000</v>
+      </c>
+      <c r="R4" s="7">
+        <v>0</v>
+      </c>
+      <c r="S4" s="7">
+        <v>0</v>
+      </c>
+      <c r="T4" s="7">
+        <v>0</v>
+      </c>
+      <c r="U4" s="8">
+        <v>1434000</v>
+      </c>
+      <c r="V4" s="9"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="K5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="7">
+        <v>618000</v>
+      </c>
+      <c r="P5" s="7">
+        <v>940000</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>62000</v>
+      </c>
+      <c r="R5" s="7">
+        <v>0</v>
+      </c>
+      <c r="S5" s="7">
+        <v>0</v>
+      </c>
+      <c r="T5" s="7">
+        <v>0</v>
+      </c>
+      <c r="U5" s="8">
+        <v>1620000</v>
+      </c>
+      <c r="V5" s="9"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="7">
+        <v>378000</v>
+      </c>
+      <c r="P6" s="7">
+        <v>820000</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>38000</v>
+      </c>
+      <c r="R6" s="7">
+        <v>0</v>
+      </c>
+      <c r="S6" s="7">
+        <v>0</v>
+      </c>
+      <c r="T6" s="7">
+        <v>0</v>
+      </c>
+      <c r="U6" s="8">
+        <v>1236000</v>
+      </c>
+      <c r="V6" s="9"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O7" s="7">
+        <v>418000</v>
+      </c>
+      <c r="P7" s="7">
+        <v>940000</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>42000</v>
+      </c>
+      <c r="R7" s="7">
+        <v>0</v>
+      </c>
+      <c r="S7" s="7">
+        <v>0</v>
+      </c>
+      <c r="T7" s="7">
+        <v>0</v>
+      </c>
+      <c r="U7" s="8">
+        <v>1400000</v>
+      </c>
+      <c r="V7" s="9"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="M8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="5" t="s">
+      <c r="N8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8" s="7">
+        <v>318000</v>
+      </c>
+      <c r="P8" s="7">
+        <v>940000</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>32000</v>
+      </c>
+      <c r="R8" s="7">
+        <v>0</v>
+      </c>
+      <c r="S8" s="7">
+        <v>0</v>
+      </c>
+      <c r="T8" s="7">
+        <v>0</v>
+      </c>
+      <c r="U8" s="8">
+        <v>1290000</v>
+      </c>
+      <c r="V8" s="9"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="7">
-        <v>418000</v>
-      </c>
-      <c r="P4" s="7">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" s="7">
+        <v>288000</v>
+      </c>
+      <c r="P9" s="7">
+        <v>820000</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>29000</v>
+      </c>
+      <c r="R9" s="7">
+        <v>0</v>
+      </c>
+      <c r="S9" s="7">
+        <v>0</v>
+      </c>
+      <c r="T9" s="7">
+        <v>0</v>
+      </c>
+      <c r="U9" s="8">
+        <v>1137000</v>
+      </c>
+      <c r="V9" s="9"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" s="7">
+        <v>318000</v>
+      </c>
+      <c r="P10" s="7">
         <v>940000</v>
       </c>
-      <c r="Q4" s="7">
-        <v>42000</v>
-      </c>
-      <c r="R4" s="7">
-        <v>120000</v>
-      </c>
-      <c r="S4" s="7">
-        <v>100000</v>
-      </c>
-      <c r="T4" s="7">
-        <v>150000</v>
-      </c>
-      <c r="U4" s="8">
-        <v>1770000</v>
-      </c>
-      <c r="V4" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="Q10" s="7">
+        <v>32000</v>
+      </c>
+      <c r="R10" s="7">
+        <v>0</v>
+      </c>
+      <c r="S10" s="7">
+        <v>0</v>
+      </c>
+      <c r="T10" s="7">
+        <v>0</v>
+      </c>
+      <c r="U10" s="8">
+        <v>1290000</v>
+      </c>
+      <c r="V10" s="9"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" s="7">
+        <v>288000</v>
+      </c>
+      <c r="P11" s="7">
+        <v>820000</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>29000</v>
+      </c>
+      <c r="R11" s="7">
+        <v>0</v>
+      </c>
+      <c r="S11" s="7">
+        <v>0</v>
+      </c>
+      <c r="T11" s="7">
+        <v>0</v>
+      </c>
+      <c r="U11" s="8">
+        <v>1137000</v>
+      </c>
+      <c r="V11" s="9"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O12" s="7">
+        <v>518000</v>
+      </c>
+      <c r="P12" s="7">
+        <v>940000</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>52000</v>
+      </c>
+      <c r="R12" s="7">
+        <v>0</v>
+      </c>
+      <c r="S12" s="7">
+        <v>0</v>
+      </c>
+      <c r="T12" s="7">
+        <v>0</v>
+      </c>
+      <c r="U12" s="8">
+        <v>1510000</v>
+      </c>
+      <c r="V12" s="9"/>
     </row>
   </sheetData>
   <mergeCells>

</xml_diff>